<commit_message>
Write to evaluation of solution and fix some paragraph in doc
</commit_message>
<xml_diff>
--- a/documentacion/analisis-evaluacion-memoria/output.xlsx
+++ b/documentacion/analisis-evaluacion-memoria/output.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GDesktop\JupyterNotebooks\analisis-evaluacion-memoria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsanh\Desktop\Memoria\documentacion\analisis-evaluacion-memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05585432-E2F2-4B9A-B9EA-8EF8D5D4D39A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F485D9-6FD4-456D-8EC7-FE68FC87151A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="functionality" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="other_app" sheetId="4" r:id="rId4"/>
     <sheet name="utility_manual" sheetId="5" r:id="rId5"/>
     <sheet name="other_manual" sheetId="6" r:id="rId6"/>
+    <sheet name="Hoja2" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -426,7 +427,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -435,13 +436,18 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-70E1-4511-94B4-738FA8B3804B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -461,7 +467,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -470,13 +476,18 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-70E1-4511-94B4-738FA8B3804B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -485,6 +496,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-70E1-4511-94B4-738FA8B3804B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -500,6 +516,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-70E1-4511-94B4-738FA8B3804B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -526,7 +547,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -646,10 +667,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.63682145131646395"/>
-          <c:y val="0.394842858688013"/>
-          <c:w val="0.20424020902260059"/>
-          <c:h val="0.21157286199992892"/>
+          <c:x val="0.64767188714615231"/>
+          <c:y val="0.22683946785447739"/>
+          <c:w val="0.28484382317441781"/>
+          <c:h val="0.37957621061526864"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -665,7 +686,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -859,6 +880,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7794-4886-B2A8-48B9823C342B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -874,6 +900,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-7794-4886-B2A8-48B9823C342B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -889,6 +920,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-7794-4886-B2A8-48B9823C342B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -1045,10 +1081,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.58602587373112358"/>
-          <c:y val="0.38586673130835963"/>
-          <c:w val="0.26638758254483069"/>
-          <c:h val="0.29960250391498833"/>
+          <c:x val="0.63050401019590441"/>
+          <c:y val="0.21897820831232895"/>
+          <c:w val="0.30682225205826796"/>
+          <c:h val="0.4948975840167264"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1064,7 +1100,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1235,6 +1271,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8E33-4FE2-86DC-2FA985CEF11F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1250,6 +1291,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8E33-4FE2-86DC-2FA985CEF11F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1265,6 +1311,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8E33-4FE2-86DC-2FA985CEF11F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1442,10 +1493,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66636558314103056"/>
-          <c:y val="0.40648123792998808"/>
+          <c:x val="0.67511591185514253"/>
+          <c:y val="0.24629293825636284"/>
           <c:w val="0.28824049102495924"/>
-          <c:h val="0.26501942441986426"/>
+          <c:h val="0.49430869938991395"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1461,7 +1512,911 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>Utilidad del manual de usuario</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001A-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001C-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>functionality!$C$17:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Totalmente en desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>En desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ni de acuerdo ni en desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>De acuerdo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Totalmente de acuerdo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>functionality!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-DC79-462B-92E3-0DA44EEB56CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-DC79-462B-92E3-0DA44EEB56CA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-DC79-462B-92E3-0DA44EEB56CA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-DC79-462B-92E3-0DA44EEB56CA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>utility_manual!$C$17:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Totalmente en desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>En desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ni de acuerdo ni en desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>De acuerdo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Totalmente de acuerdo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>utility_manual!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-DC79-462B-92E3-0DA44EEB56CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.67511591185514253"/>
+          <c:y val="0.24629293825636284"/>
+          <c:w val="0.28824049102495924"/>
+          <c:h val="0.49430869938991395"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Utilidad</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Serie</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8F89-40B4-B8AE-86A55044E41C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8F89-40B4-B8AE-86A55044E41C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8F89-40B4-B8AE-86A55044E41C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8F89-40B4-B8AE-86A55044E41C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-8F89-40B4-B8AE-86A55044E41C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-8F89-40B4-B8AE-86A55044E41C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-8F89-40B4-B8AE-86A55044E41C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>utility!$C$17:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Totalmente en desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>En desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ni de acuerdo ni en desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>De acuerdo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Totalmente de acuerdo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>utility!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-8F89-40B4-B8AE-86A55044E41C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.63050401019590441"/>
+          <c:y val="0.21897820831232895"/>
+          <c:w val="0.30682225205826796"/>
+          <c:h val="0.4948975840167264"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1517,6 +2472,418 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>Utilidad del manual de usuario</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7C7E-4C6A-B532-AE41EE2284BA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7C7E-4C6A-B532-AE41EE2284BA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7C7E-4C6A-B532-AE41EE2284BA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-7C7E-4C6A-B532-AE41EE2284BA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-7C7E-4C6A-B532-AE41EE2284BA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-7C7E-4C6A-B532-AE41EE2284BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-7C7E-4C6A-B532-AE41EE2284BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>utility_manual!$C$17:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Totalmente en desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>En desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ni de acuerdo ni en desacuerdo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>De acuerdo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Totalmente de acuerdo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>utility_manual!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-7C7E-4C6A-B532-AE41EE2284BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.67511591185514253"/>
+          <c:y val="0.24629293825636284"/>
+          <c:w val="0.28824049102495924"/>
+          <c:h val="0.49430869938991395"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1641,6 +3008,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -2680,6 +4127,1044 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3203,15 +5688,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>918881</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>530819</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:rowOff>53662</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3246,13 +5731,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>395287</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:rowOff>166685</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>280087</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>63185</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3285,15 +5770,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>442911</xdr:colOff>
+      <xdr:colOff>442910</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>327710</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>63186</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3313,6 +5798,125 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>532500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>134625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ADAC566-ACFD-4C99-A536-770615B7FAF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>465825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>87000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63581A22-45B9-41F2-963F-9C70E17ACCE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>513450</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>20325</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{080DEE01-DC2D-436A-A925-5EFB379C1BFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3641,8 +6245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D22"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3655,7 +6259,7 @@
     <col min="23" max="23" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4010,7 +6614,7 @@
         <v>Ni de acuerdo ni en desacuerdo</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" ref="D9:D12" si="2">COUNTIF(D$2:D$4,$U10)</f>
+        <f t="shared" ref="D10:D12" si="2">COUNTIF(D$2:D$4,$U10)</f>
         <v>0</v>
       </c>
       <c r="E10" s="5">
@@ -4346,7 +6950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -4527,7 +7131,7 @@
         <v>2</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O3:O4" si="0">((D4-1)+(F4-1)+(H4-1)+(J4-1)+(L4-1)+(5-E4)+(5-G4)+(5-I4)+(5-K4)+(5-M4))*2.5</f>
+        <f t="shared" ref="O4" si="0">((D4-1)+(F4-1)+(H4-1)+(J4-1)+(L4-1)+(5-E4)+(5-G4)+(5-I4)+(5-K4)+(5-M4))*2.5</f>
         <v>90</v>
       </c>
     </row>
@@ -4561,7 +7165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
@@ -5161,8 +7765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5316,7 +7920,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" ref="E8:N12" si="1">COUNTIF(E$2:E$4,$U9)</f>
+        <f t="shared" ref="E9:F12" si="1">COUNTIF(E$2:E$4,$U9)</f>
         <v>1</v>
       </c>
       <c r="F9" s="5">
@@ -5464,7 +8068,7 @@
         <v>En desacuerdo</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" ref="D18:D22" si="3">SUM($D9:$F9)</f>
+        <f t="shared" ref="D18:D21" si="3">SUM($D9:$F9)</f>
         <v>2</v>
       </c>
     </row>
@@ -5535,7 +8139,7 @@
     <col min="5" max="5" width="168.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5607,4 +8211,20 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FEE4B2-44A8-4381-A684-E0767722D6EA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>